<commit_message>
add manual test case and daily tracker documentation
</commit_message>
<xml_diff>
--- a/postman_rest_api/API Manual Test Sheet/Mini project api doct.xlsx
+++ b/postman_rest_api/API Manual Test Sheet/Mini project api doct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mini_Project_2021\postman_rest_api\API Manual Test Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4824F4-6769-4D18-A475-5EACC19EAB37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF8A0B1-7818-4C48-96F7-792AADEC4E20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A2B6A8C2-190E-41B6-A56A-5A40BFF8A5C2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{A2B6A8C2-190E-41B6-A56A-5A40BFF8A5C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin Authorization" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="225">
   <si>
     <t>Modules</t>
   </si>
@@ -992,6 +992,10 @@
   <si>
     <t>Organization details with
 wrong information</t>
+  </si>
+  <si>
+    <t>time period when
+employee gets leave</t>
   </si>
 </sst>
 </file>
@@ -1440,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A1BF19-49C2-44C3-8562-47A161B2C8CD}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1781,7 +1785,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="C18" sqref="C18:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2935,8 +2939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71930C1A-DA7A-4881-8AA6-E3A71BECCCBB}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3074,7 +3078,9 @@
       <c r="B4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="14" t="s">
+        <v>224</v>
+      </c>
       <c r="D4" s="8" t="s">
         <v>19</v>
       </c>
@@ -3187,7 +3193,9 @@
       <c r="D7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="F7" s="12" t="s">
         <v>79</v>
       </c>
@@ -3290,8 +3298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCFFAE2-522E-42A9-ABE7-5B7F996238A2}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>